<commit_message>
Fim do trabalho 3
</commit_message>
<xml_diff>
--- a/trabalho 3/valores.xlsx
+++ b/trabalho 3/valores.xlsx
@@ -75,6 +75,754 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>MSE</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> e PSNR</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MSE</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Mean!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Mean!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>47.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>PSNR</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Mean!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>27.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="68016000"/>
+        <c:axId val="68292992"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="68016000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Número</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> de Imagens</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68292992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="68292992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68016000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SSIM</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Mean!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Mean!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.84599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98899999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="68317184"/>
+        <c:axId val="68319104"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="68317184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Número de Imagens</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68319104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="68319104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68317184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>MSE</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> e PSNR</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MSE</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adaptive Mean'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adaptive Mean'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>48.37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.340000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>PSNR</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adaptive Mean'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adaptive Mean'!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>26.74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="70621824"/>
+        <c:axId val="70640384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="70621824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Máscara</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70640384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="70640384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70621824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SSIM</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Adaptive Mean'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Adaptive Mean'!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.73199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82299999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="68706688"/>
+        <c:axId val="68708608"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="68706688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Máscara</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68708608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="68708608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68706688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -365,7 +1113,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -445,6 +1193,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -453,7 +1202,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -474,16 +1223,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>62.39</v>
+        <v>48.37</v>
       </c>
       <c r="C2">
-        <v>0.64400000000000002</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="D2">
-        <v>23.84</v>
+        <v>26.74</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -491,45 +1240,46 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>35.380000000000003</v>
+        <v>35.340000000000003</v>
       </c>
       <c r="C3">
-        <v>0.81200000000000006</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="D3">
-        <v>27.89</v>
+        <v>27.88</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>36.090000000000003</v>
+        <v>33.28</v>
       </c>
       <c r="C4">
-        <v>0.79500000000000004</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="D4">
-        <v>24.98</v>
+        <v>27.18</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>43.53</v>
+        <v>34.17</v>
       </c>
       <c r="C5">
-        <v>0.73899999999999999</v>
+        <v>0.81</v>
       </c>
       <c r="D5">
-        <v>24.13</v>
+        <v>26.34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>